<commit_message>
Fixed writing to spreadsheet
</commit_message>
<xml_diff>
--- a/coronaTracker.xlsx
+++ b/coronaTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbryan/github/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20212B32-2275-304B-8E8B-25D0E40CFA00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEF4462-92E4-564C-82F5-BF4CD83D4437}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
   <si>
     <t>Hubei province (includes Wuhan)</t>
   </si>
@@ -220,6 +220,15 @@
     <t>Mexico</t>
   </si>
   <si>
+    <t>Cases</t>
+  </si>
+  <si>
+    <t>Deaths</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>7,633 serious</t>
   </si>
   <si>
@@ -238,7 +247,7 @@
     <t>9 serious, 3 critical</t>
   </si>
   <si>
-    <t>133 serious/critical</t>
+    <t>141 serious/critical</t>
   </si>
   <si>
     <t>34 serious, 10 recovered</t>
@@ -247,7 +256,7 @@
     <t>7 critical, 24 recovered</t>
   </si>
   <si>
-    <t xml:space="preserve">56 serious, 45 recovered </t>
+    <t xml:space="preserve">64 serious, 46 recovered </t>
   </si>
   <si>
     <t>13 serious, 32 recovered</t>
@@ -302,21 +311,6 @@
   </si>
   <si>
     <t>1 recovered</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Cases</t>
-  </si>
-  <si>
-    <t>Deaths</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -665,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -674,14 +668,14 @@
     <col min="1" max="2" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:68" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -886,7 +880,7 @@
     </row>
     <row r="2" spans="1:68" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1">
         <v>65914</v>
@@ -913,7 +907,7 @@
         <v>7321</v>
       </c>
       <c r="J2" s="1">
-        <v>5055</v>
+        <v>5288</v>
       </c>
       <c r="K2" s="1">
         <v>705</v>
@@ -922,7 +916,7 @@
         <v>2337</v>
       </c>
       <c r="M2" s="1">
-        <v>655</v>
+        <v>888</v>
       </c>
       <c r="N2" s="3">
         <v>226</v>
@@ -1089,7 +1083,7 @@
     </row>
     <row r="3" spans="1:68" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3">
         <v>2682</v>
@@ -1116,7 +1110,7 @@
         <v>64</v>
       </c>
       <c r="J3" s="1">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="K3" s="1">
         <v>6</v>
@@ -1125,7 +1119,7 @@
         <v>16</v>
       </c>
       <c r="M3" s="1">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="N3" s="1">
         <v>5</v>
@@ -1295,142 +1289,158 @@
     </row>
     <row r="4" spans="1:68" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="G4"/>
       <c r="H4" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="I4"/>
       <c r="J4" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="U4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
       <c r="AG4" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="AK4"/>
       <c r="AL4" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="AP4"/>
       <c r="AQ4" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="AS4"/>
+      <c r="AT4"/>
+      <c r="AU4"/>
+      <c r="AV4"/>
+      <c r="AW4"/>
+      <c r="AX4"/>
+      <c r="AY4"/>
+      <c r="AZ4"/>
+      <c r="BA4"/>
+      <c r="BB4"/>
+      <c r="BC4"/>
+      <c r="BD4"/>
+      <c r="BE4"/>
+      <c r="BF4"/>
+      <c r="BG4"/>
+      <c r="BH4"/>
+      <c r="BI4"/>
+      <c r="BJ4"/>
+      <c r="BK4"/>
+      <c r="BL4"/>
+      <c r="BM4"/>
+      <c r="BN4"/>
+      <c r="BO4"/>
     </row>
-    <row r="22" spans="18:21" x14ac:dyDescent="0.2">
-      <c r="S22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="T22" t="s">
-        <v>95</v>
-      </c>
-      <c r="U22" t="s">
-        <v>12</v>
-      </c>
+    <row r="22" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="18:21" x14ac:dyDescent="0.2">
-      <c r="R23" s="1" t="s">
-        <v>96</v>
-      </c>
+    <row r="23" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="18:21" x14ac:dyDescent="0.2">
-      <c r="R24" s="1" t="s">
-        <v>97</v>
-      </c>
+    <row r="24" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="18:21" x14ac:dyDescent="0.2">
-      <c r="R25" s="1" t="s">
-        <v>98</v>
-      </c>
+    <row r="25" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>